<commit_message>
added average attack distances
</commit_message>
<xml_diff>
--- a/attacks.xlsx
+++ b/attacks.xlsx
@@ -1,46 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="all_binned_counts" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -48,21 +45,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -350,14 +420,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
+    <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>period_id</t>
@@ -403,9 +479,14 @@
           <t>Other</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>avg_distance_km</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
@@ -423,24 +504,27 @@
           <t>2023-10-07 to 2023-10-20</t>
         </is>
       </c>
-      <c r="E2">
+      <c r="E2" t="n">
         <v>374</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="n">
         <v>5</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="n">
         <v>67</v>
       </c>
-      <c r="H2">
+      <c r="H2" t="n">
         <v>1</v>
       </c>
-      <c r="I2">
+      <c r="I2" t="n">
         <v>4</v>
       </c>
+      <c r="J2" t="n">
+        <v>3.76326812791891</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3">
+      <c r="A3" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
@@ -458,24 +542,27 @@
           <t>2023-10-21 to 2023-11-03</t>
         </is>
       </c>
-      <c r="E3">
+      <c r="E3" t="n">
         <v>374</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="n">
         <v>67</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="n">
         <v>211</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="n">
         <v>1</v>
       </c>
-      <c r="I3">
+      <c r="I3" t="n">
         <v>3</v>
       </c>
+      <c r="J3" t="n">
+        <v>4.385888662670677</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4">
+      <c r="A4" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
@@ -493,24 +580,27 @@
           <t>2023-12-11 to 2023-12-24</t>
         </is>
       </c>
-      <c r="E4">
+      <c r="E4" t="n">
         <v>260</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="n">
         <v>137</v>
       </c>
-      <c r="G4">
+      <c r="G4" t="n">
         <v>238</v>
       </c>
-      <c r="H4">
+      <c r="H4" t="n">
         <v>17</v>
       </c>
-      <c r="I4">
+      <c r="I4" t="n">
         <v>0</v>
       </c>
+      <c r="J4" t="n">
+        <v>4.11879765724225</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5">
+      <c r="A5" t="n">
         <v>2</v>
       </c>
       <c r="B5" t="inlineStr">
@@ -528,24 +618,27 @@
           <t>2023-12-25 to 2024-01-07</t>
         </is>
       </c>
-      <c r="E5">
+      <c r="E5" t="n">
         <v>243</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="n">
         <v>97</v>
       </c>
-      <c r="G5">
+      <c r="G5" t="n">
         <v>264</v>
       </c>
-      <c r="H5">
+      <c r="H5" t="n">
         <v>15</v>
       </c>
-      <c r="I5">
+      <c r="I5" t="n">
         <v>4</v>
       </c>
+      <c r="J5" t="n">
+        <v>4.897854013092467</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6">
+      <c r="A6" t="n">
         <v>2</v>
       </c>
       <c r="B6" t="inlineStr">
@@ -563,24 +656,27 @@
           <t>2024-01-08 to 2024-01-21</t>
         </is>
       </c>
-      <c r="E6">
+      <c r="E6" t="n">
         <v>246</v>
       </c>
-      <c r="F6">
+      <c r="F6" t="n">
         <v>124</v>
       </c>
-      <c r="G6">
+      <c r="G6" t="n">
         <v>242</v>
       </c>
-      <c r="H6">
+      <c r="H6" t="n">
         <v>33</v>
       </c>
-      <c r="I6">
+      <c r="I6" t="n">
         <v>0</v>
       </c>
+      <c r="J6" t="n">
+        <v>4.476229029663664</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7">
+      <c r="A7" t="n">
         <v>2</v>
       </c>
       <c r="B7" t="inlineStr">
@@ -598,24 +694,27 @@
           <t>2024-01-22 to 2024-02-04</t>
         </is>
       </c>
-      <c r="E7">
+      <c r="E7" t="n">
         <v>206</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="n">
         <v>106</v>
       </c>
-      <c r="G7">
+      <c r="G7" t="n">
         <v>234</v>
       </c>
-      <c r="H7">
+      <c r="H7" t="n">
         <v>39</v>
       </c>
-      <c r="I7">
+      <c r="I7" t="n">
         <v>1</v>
       </c>
+      <c r="J7" t="n">
+        <v>3.876734017006266</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8">
+      <c r="A8" t="n">
         <v>2</v>
       </c>
       <c r="B8" t="inlineStr">
@@ -633,24 +732,27 @@
           <t>2024-02-05 to 2024-02-18</t>
         </is>
       </c>
-      <c r="E8">
+      <c r="E8" t="n">
         <v>260</v>
       </c>
-      <c r="F8">
+      <c r="F8" t="n">
         <v>76</v>
       </c>
-      <c r="G8">
+      <c r="G8" t="n">
         <v>161</v>
       </c>
-      <c r="H8">
+      <c r="H8" t="n">
         <v>31</v>
       </c>
-      <c r="I8">
+      <c r="I8" t="n">
         <v>3</v>
       </c>
+      <c r="J8" t="n">
+        <v>3.709505535754547</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9">
+      <c r="A9" t="n">
         <v>2</v>
       </c>
       <c r="B9" t="inlineStr">
@@ -668,24 +770,27 @@
           <t>2024-02-19 to 2024-03-03</t>
         </is>
       </c>
-      <c r="E9">
+      <c r="E9" t="n">
         <v>241</v>
       </c>
-      <c r="F9">
+      <c r="F9" t="n">
         <v>55</v>
       </c>
-      <c r="G9">
+      <c r="G9" t="n">
         <v>231</v>
       </c>
-      <c r="H9">
+      <c r="H9" t="n">
         <v>22</v>
       </c>
-      <c r="I9">
+      <c r="I9" t="n">
         <v>0</v>
       </c>
+      <c r="J9" t="n">
+        <v>4.299951632670066</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10">
+      <c r="A10" t="n">
         <v>2</v>
       </c>
       <c r="B10" t="inlineStr">
@@ -703,24 +808,27 @@
           <t>2024-03-04 to 2024-03-17</t>
         </is>
       </c>
-      <c r="E10">
+      <c r="E10" t="n">
         <v>246</v>
       </c>
-      <c r="F10">
+      <c r="F10" t="n">
         <v>37</v>
       </c>
-      <c r="G10">
+      <c r="G10" t="n">
         <v>231</v>
       </c>
-      <c r="H10">
+      <c r="H10" t="n">
         <v>18</v>
       </c>
-      <c r="I10">
+      <c r="I10" t="n">
         <v>1</v>
       </c>
+      <c r="J10" t="n">
+        <v>4.675176933039502</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11">
+      <c r="A11" t="n">
         <v>2</v>
       </c>
       <c r="B11" t="inlineStr">
@@ -738,24 +846,27 @@
           <t>2024-03-18 to 2024-03-31</t>
         </is>
       </c>
-      <c r="E11">
+      <c r="E11" t="n">
         <v>243</v>
       </c>
-      <c r="F11">
+      <c r="F11" t="n">
         <v>66</v>
       </c>
-      <c r="G11">
+      <c r="G11" t="n">
         <v>204</v>
       </c>
-      <c r="H11">
+      <c r="H11" t="n">
         <v>17</v>
       </c>
-      <c r="I11">
+      <c r="I11" t="n">
         <v>2</v>
       </c>
+      <c r="J11" t="n">
+        <v>4.286881911154486</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12">
+      <c r="A12" t="n">
         <v>2</v>
       </c>
       <c r="B12" t="inlineStr">
@@ -773,24 +884,27 @@
           <t>2024-04-01 to 2024-04-14</t>
         </is>
       </c>
-      <c r="E12">
+      <c r="E12" t="n">
         <v>182</v>
       </c>
-      <c r="F12">
+      <c r="F12" t="n">
         <v>32</v>
       </c>
-      <c r="G12">
+      <c r="G12" t="n">
         <v>181</v>
       </c>
-      <c r="H12">
+      <c r="H12" t="n">
         <v>15</v>
       </c>
-      <c r="I12">
+      <c r="I12" t="n">
         <v>10</v>
       </c>
+      <c r="J12" t="n">
+        <v>4.541151156676015</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13">
+      <c r="A13" t="n">
         <v>2</v>
       </c>
       <c r="B13" t="inlineStr">
@@ -808,24 +922,27 @@
           <t>2024-04-15 to 2024-04-28</t>
         </is>
       </c>
-      <c r="E13">
+      <c r="E13" t="n">
         <v>248</v>
       </c>
-      <c r="F13">
+      <c r="F13" t="n">
         <v>25</v>
       </c>
-      <c r="G13">
+      <c r="G13" t="n">
         <v>157</v>
       </c>
-      <c r="H13">
+      <c r="H13" t="n">
         <v>9</v>
       </c>
-      <c r="I13">
+      <c r="I13" t="n">
         <v>7</v>
       </c>
+      <c r="J13" t="n">
+        <v>4.723351366358533</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14">
+      <c r="A14" t="n">
         <v>3</v>
       </c>
       <c r="B14" t="inlineStr">
@@ -843,24 +960,27 @@
           <t>2024-11-11 to 2024-11-24</t>
         </is>
       </c>
-      <c r="E14">
+      <c r="E14" t="n">
         <v>210</v>
       </c>
-      <c r="F14">
+      <c r="F14" t="n">
         <v>35</v>
       </c>
-      <c r="G14">
+      <c r="G14" t="n">
         <v>182</v>
       </c>
-      <c r="H14">
+      <c r="H14" t="n">
         <v>38</v>
       </c>
-      <c r="I14">
+      <c r="I14" t="n">
         <v>6</v>
       </c>
+      <c r="J14" t="n">
+        <v>4.561800693261488</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15">
+      <c r="A15" t="n">
         <v>3</v>
       </c>
       <c r="B15" t="inlineStr">
@@ -878,24 +998,27 @@
           <t>2024-11-25 to 2024-12-08</t>
         </is>
       </c>
-      <c r="E15">
+      <c r="E15" t="n">
         <v>207</v>
       </c>
-      <c r="F15">
+      <c r="F15" t="n">
         <v>24</v>
       </c>
-      <c r="G15">
+      <c r="G15" t="n">
         <v>132</v>
       </c>
-      <c r="H15">
+      <c r="H15" t="n">
         <v>55</v>
       </c>
-      <c r="I15">
+      <c r="I15" t="n">
         <v>0</v>
       </c>
+      <c r="J15" t="n">
+        <v>4.508389709238768</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16">
+      <c r="A16" t="n">
         <v>3</v>
       </c>
       <c r="B16" t="inlineStr">
@@ -913,24 +1036,27 @@
           <t>2024-12-09 to 2024-12-22</t>
         </is>
       </c>
-      <c r="E16">
+      <c r="E16" t="n">
         <v>225</v>
       </c>
-      <c r="F16">
+      <c r="F16" t="n">
         <v>25</v>
       </c>
-      <c r="G16">
+      <c r="G16" t="n">
         <v>101</v>
       </c>
-      <c r="H16">
+      <c r="H16" t="n">
         <v>57</v>
       </c>
-      <c r="I16">
+      <c r="I16" t="n">
         <v>1</v>
       </c>
+      <c r="J16" t="n">
+        <v>4.518039712920642</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17">
+      <c r="A17" t="n">
         <v>3</v>
       </c>
       <c r="B17" t="inlineStr">
@@ -948,24 +1074,27 @@
           <t>2024-12-23 to 2025-01-05</t>
         </is>
       </c>
-      <c r="E17">
+      <c r="E17" t="n">
         <v>237</v>
       </c>
-      <c r="F17">
+      <c r="F17" t="n">
         <v>22</v>
       </c>
-      <c r="G17">
+      <c r="G17" t="n">
         <v>107</v>
       </c>
-      <c r="H17">
+      <c r="H17" t="n">
         <v>40</v>
       </c>
-      <c r="I17">
+      <c r="I17" t="n">
         <v>0</v>
       </c>
+      <c r="J17" t="n">
+        <v>4.490206231553414</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18">
+      <c r="A18" t="n">
         <v>3</v>
       </c>
       <c r="B18" t="inlineStr">
@@ -983,24 +1112,27 @@
           <t>2025-01-06 to 2025-01-19</t>
         </is>
       </c>
-      <c r="E18">
+      <c r="E18" t="n">
         <v>215</v>
       </c>
-      <c r="F18">
+      <c r="F18" t="n">
         <v>28</v>
       </c>
-      <c r="G18">
+      <c r="G18" t="n">
         <v>115</v>
       </c>
-      <c r="H18">
+      <c r="H18" t="n">
         <v>35</v>
       </c>
-      <c r="I18">
+      <c r="I18" t="n">
         <v>1</v>
       </c>
+      <c r="J18" t="n">
+        <v>4.171829734708102</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19">
+      <c r="A19" t="n">
         <v>3</v>
       </c>
       <c r="B19" t="inlineStr">
@@ -1018,23 +1150,26 @@
           <t>2025-01-20 to 2025-02-02</t>
         </is>
       </c>
-      <c r="E19">
+      <c r="E19" t="n">
         <v>13</v>
       </c>
-      <c r="F19">
+      <c r="F19" t="n">
         <v>27</v>
       </c>
-      <c r="G19">
+      <c r="G19" t="n">
         <v>20</v>
       </c>
-      <c r="H19">
+      <c r="H19" t="n">
         <v>5</v>
       </c>
-      <c r="I19">
+      <c r="I19" t="n">
         <v>0</v>
       </c>
+      <c r="J19" t="n">
+        <v>4.136376498618044</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>